<commit_message>
All Result ready to start write
</commit_message>
<xml_diff>
--- a/EL/estimated_100genes_weakILS_EL_Phylonet100_FNRATE_ASTRAL.xlsx
+++ b/EL/estimated_100genes_weakILS_EL_Phylonet100_FNRATE_ASTRAL.xlsx
@@ -25,7 +25,7 @@
     <t>TAXON</t>
   </si>
   <si>
-    <t>MODEL_CONDITION</t>
+    <t>MODELCONDITION</t>
   </si>
   <si>
     <t>GENE</t>
@@ -392,66 +392,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>338</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>11</v>
-      </c>
-      <c r="B2">
+    <row r="3" spans="1:5">
+      <c r="A3">
         <v>338</v>
       </c>
-      <c r="C2">
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="F2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>338</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3">
+      <c r="E3">
         <v>17</v>
       </c>
     </row>

</xml_diff>